<commit_message>
Añadidos el resto de archivos
Añadidos archivos para completar la subida a GitHub y que no falte ninguna dependencia
</commit_message>
<xml_diff>
--- a/dataset_excel/dentro_rotonda_test.xlsx
+++ b/dataset_excel/dentro_rotonda_test.xlsx
@@ -990,7 +990,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1423,12 +1423,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>quito intermitente</t>
+          <t>salgo rotonda</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BLK-OFF</t>
+          <t>RND-EXIT</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -1438,17 +1438,17 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6558634638786316</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.06250572204589844</v>
+        <v>-0.800000011920929</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>NONE</t>
+          <t>Right_Blinker</t>
         </is>
       </c>
       <c r="I9" t="b">
@@ -1458,116 +1458,16 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L9" t="n">
-        <v>10.9213399887085</v>
+        <v>11.56580257415771</v>
       </c>
       <c r="M9" t="n">
-        <v>-34.34526443481445</v>
+        <v>-19.83598136901855</v>
       </c>
       <c r="N9" t="n">
-        <v>0.00170900346711278</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>sigo recto</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>STR</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>4</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.8500000238418579</v>
-      </c>
-      <c r="F10" t="n">
-        <v>-0.09303539991378784</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>43</v>
-      </c>
-      <c r="L10" t="n">
-        <v>9.720303535461426</v>
-      </c>
-      <c r="M10" t="n">
-        <v>-41.79500579833984</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.001697521191090345</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>acelero</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>T-ON</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>4</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.6114190220832825</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.02058845013380051</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>47</v>
-      </c>
-      <c r="L11" t="n">
-        <v>8.383475303649902</v>
-      </c>
-      <c r="M11" t="n">
-        <v>-50.03433609008789</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.001722583780065179</v>
+        <v>0.002488384256139398</v>
       </c>
     </row>
   </sheetData>
@@ -1822,7 +1722,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2055,12 +1955,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>intermitente derecha</t>
+          <t>quito intermitente</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RB-ON</t>
+          <t>BLK-OFF</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -2070,10 +1970,10 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8500000238418579</v>
+        <v>0.5020059943199158</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5637196898460388</v>
+        <v>-0.2378262132406235</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -2093,24 +1993,24 @@
         <v>41</v>
       </c>
       <c r="L5" t="n">
-        <v>-21.08345603942871</v>
+        <v>-20.16416549682617</v>
       </c>
       <c r="M5" t="n">
-        <v>-2.517086029052734</v>
+        <v>-7.858899593353271</v>
       </c>
       <c r="N5" t="n">
-        <v>0.001879749237559736</v>
+        <v>0.001834316179156303</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>giro derecha</t>
+          <t>intermitente derecha</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TURN-R</t>
+          <t>RB-ON</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -2123,14 +2023,14 @@
         <v>0.8500000238418579</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7715815305709839</v>
+        <v>0.5637196898460388</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Right_Blinker</t>
+          <t>Left_Blinker</t>
         </is>
       </c>
       <c r="I6" t="b">
@@ -2140,27 +2040,27 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="L6" t="n">
-        <v>-16.63599014282227</v>
+        <v>-21.08345603942871</v>
       </c>
       <c r="M6" t="n">
-        <v>10.20130252838135</v>
+        <v>-2.517086029052734</v>
       </c>
       <c r="N6" t="n">
-        <v>0.002073078183457255</v>
+        <v>0.001879749237559736</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>salgo rotonda</t>
+          <t>giro derecha</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RND-EXIT</t>
+          <t>TURN-R</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -2170,35 +2070,85 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.7715815305709839</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>32</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-16.63599014282227</v>
+      </c>
+      <c r="M7" t="n">
+        <v>10.20130252838135</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.002073078183457255</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>salgo rotonda</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>RND-EXIT</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
         <v>0.2796191573143005</v>
       </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="inlineStr">
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
         <v>27</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L8" t="n">
         <v>-14.00700569152832</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M8" t="n">
         <v>14.32025718688965</v>
       </c>
-      <c r="N7" t="n">
+      <c r="N8" t="n">
         <v>0.002015819540247321</v>
       </c>
     </row>
@@ -2546,7 +2496,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>gira derecha</t>
+          <t>giro derecha</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2887,7 +2837,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>gira izquierda</t>
+          <t>giro izquierda</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3528,7 +3478,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>gira derecha</t>
+          <t>giro derecha</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">

</xml_diff>